<commit_message>
UI changes in GUA
</commit_message>
<xml_diff>
--- a/MyBlock/resources/TestData.xlsx
+++ b/MyBlock/resources/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="427">
   <si>
     <t>Username</t>
   </si>
@@ -1322,6 +1322,9 @@
   </si>
   <si>
     <t>Tc_940175_UploadDocOf10MBValidateTY2016</t>
+  </si>
+  <si>
+    <t>ms022316</t>
   </si>
 </sst>
 </file>
@@ -2810,8 +2813,8 @@
   <dimension ref="A1:BE263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B263" sqref="B263:C263"/>
+      <pane ySplit="2" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B249" sqref="B249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7830,8 +7833,8 @@
       <c r="A249" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="B249" s="8" t="s">
-        <v>107</v>
+      <c r="B249" s="51" t="s">
+        <v>426</v>
       </c>
       <c r="C249" s="8" t="s">
         <v>4</v>

</xml_diff>